<commit_message>
added new powerups - "Safety Net"
</commit_message>
<xml_diff>
--- a/Bricks/BrickBreacker Probability Table.xlsx
+++ b/Bricks/BrickBreacker Probability Table.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="30">
   <si>
     <t>Powerup</t>
   </si>
@@ -111,6 +111,9 @@
   </si>
   <si>
     <t>Low Collision Amounts</t>
+  </si>
+  <si>
+    <t>Safety Net</t>
   </si>
 </sst>
 </file>
@@ -479,8 +482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AD25"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="U2" sqref="U2"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="U24" sqref="U24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1326,14 +1329,42 @@
       <c r="AD23" s="9"/>
     </row>
     <row r="24" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="B24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="J24" s="1"/>
-      <c r="N24" s="1"/>
-      <c r="Q24" s="2"/>
-      <c r="R24" s="3"/>
-      <c r="U24" s="2"/>
-      <c r="V24" s="3"/>
+      <c r="A24" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" s="1">
+        <v>0.04</v>
+      </c>
+      <c r="E24" t="s">
+        <v>29</v>
+      </c>
+      <c r="F24" s="1">
+        <v>0.04</v>
+      </c>
+      <c r="I24" t="s">
+        <v>29</v>
+      </c>
+      <c r="J24" s="1">
+        <v>0.04</v>
+      </c>
+      <c r="M24" t="s">
+        <v>29</v>
+      </c>
+      <c r="N24" s="1">
+        <v>0.04</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>29</v>
+      </c>
+      <c r="R24" s="3">
+        <v>0.04</v>
+      </c>
+      <c r="U24" t="s">
+        <v>29</v>
+      </c>
+      <c r="V24" s="3">
+        <v>0.04</v>
+      </c>
       <c r="Y24" s="2"/>
       <c r="Z24" s="3"/>
       <c r="AC24" s="2"/>
@@ -1344,43 +1375,43 @@
         <v>22</v>
       </c>
       <c r="B25" s="7">
-        <f>SUM(B5:B23)</f>
-        <v>1.0000000000000002</v>
+        <f>SUM(B5:B24)</f>
+        <v>1.0400000000000003</v>
       </c>
       <c r="E25" s="6" t="s">
         <v>22</v>
       </c>
       <c r="F25" s="7">
-        <f>SUM(F5:F23)</f>
-        <v>1.0000000000000004</v>
+        <f>SUM(F5:F24)</f>
+        <v>1.0400000000000005</v>
       </c>
       <c r="I25" s="6" t="s">
         <v>22</v>
       </c>
       <c r="J25" s="7">
-        <f>SUM(J5:J23)</f>
-        <v>1.0000000000000004</v>
+        <f>SUM(J5:J24)</f>
+        <v>1.0400000000000005</v>
       </c>
       <c r="M25" s="6" t="s">
         <v>22</v>
       </c>
       <c r="N25" s="7">
-        <f>SUM(N5:N23)</f>
-        <v>1.0000000000000004</v>
+        <f>SUM(N5:N24)</f>
+        <v>1.0400000000000005</v>
       </c>
       <c r="Q25" s="8" t="s">
         <v>22</v>
       </c>
       <c r="R25" s="9">
-        <f>SUM(R5:R23)</f>
-        <v>1.0000000000000002</v>
+        <f>SUM(R5:R24)</f>
+        <v>1.0400000000000003</v>
       </c>
       <c r="U25" s="8" t="s">
         <v>22</v>
       </c>
       <c r="V25" s="9">
-        <f>SUM(V5:V23)</f>
-        <v>1</v>
+        <f>SUM(V5:V24)</f>
+        <v>1.04</v>
       </c>
       <c r="Y25" s="8"/>
       <c r="Z25" s="9"/>

</xml_diff>